<commit_message>
Work in progress: Adding SciNotationNum support to BigIntNum and IntAry.
</commit_message>
<xml_diff>
--- a/notes/scientificnotation/scientificnotation.xlsx
+++ b/notes/scientificnotation/scientificnotation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF46897-60E3-4DA3-BD0A-AD7D846A933C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081CF6A6-6301-4464-B925-C9F0E0C1A83D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Integers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>10^4</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t xml:space="preserve">Divide by 20 </t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>10^Precision</t>
+  </si>
+  <si>
+    <t>base x 10^Precision</t>
   </si>
 </sst>
 </file>
@@ -114,11 +123,11 @@
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000000000"/>
-    <numFmt numFmtId="171" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00000000000_);[Red]\(#,##0.00000000000\)"/>
-    <numFmt numFmtId="174" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="175" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000000000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00000000000_);[Red]\(#,##0.00000000000\)"/>
+    <numFmt numFmtId="169" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -160,12 +169,12 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,7 +1082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8798649-3A87-4212-8AB5-82733B9FDE7A}">
   <dimension ref="C2:AZ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB19" workbookViewId="0">
+    <sheetView topLeftCell="AB19" workbookViewId="0">
       <selection activeCell="AZ26" sqref="AZ26"/>
     </sheetView>
   </sheetViews>
@@ -1704,7 +1713,7 @@
         <v>1.2</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25:Q25" si="3">+F23/F24</f>
+        <f t="shared" ref="F25:P25" si="3">+F23/F24</f>
         <v>1.5</v>
       </c>
       <c r="G25">
@@ -2017,14 +2026,46 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA12BD44-8E7B-425F-9893-89E78E2C052F}">
-  <dimension ref="A1"/>
+  <dimension ref="E3:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0.123456</v>
+      </c>
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f>10^F5</f>
+        <v>1000000</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>+E7*E3</f>
+        <v>123456</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed broken BigIntNum exponent tests.
</commit_message>
<xml_diff>
--- a/notes/scientificnotation/scientificnotation.xlsx
+++ b/notes/scientificnotation/scientificnotation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FF07D3-85D5-4EB2-B591-FD9A9A504D7A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15623E46-AED8-425C-9A58-2C069E7B77AD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Integers" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="BinaryExponents" sheetId="3" r:id="rId3"/>
     <sheet name="BinaryExp-2" sheetId="4" r:id="rId4"/>
     <sheet name="BinaryExp-3" sheetId="5" r:id="rId5"/>
+    <sheet name="Multiply" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>10^4</t>
   </si>
@@ -129,6 +130,33 @@
   </si>
   <si>
     <t>Exponent should be -5</t>
+  </si>
+  <si>
+    <t>a^x * b^y</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>correct answer</t>
+  </si>
+  <si>
+    <t>x+y</t>
+  </si>
+  <si>
+    <t>a*b</t>
+  </si>
+  <si>
+    <t>(a*b)^x+y</t>
   </si>
 </sst>
 </file>
@@ -2053,7 +2081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA12BD44-8E7B-425F-9893-89E78E2C052F}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -2477,4 +2505,116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C71947-B5CB-421F-8928-074E4071C279}">
+  <dimension ref="C4:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <f>(E7^F7)*(H7^I7)</f>
+        <v>1296</v>
+      </c>
+      <c r="I11">
+        <f>+E7*H7</f>
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="M11">
+        <f>I11^K11</f>
+        <v>279936</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <f>I12^K12</f>
+        <v>1679616</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>+E7^F7</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>+H7^I7</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f>+E13*E14</f>
+        <v>1296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>